<commit_message>
Analytics: config, pass rules, disposition Excel export (formatting + borders), tray summary, clear cache
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/templates/Tray_Summary_Template.xlsx
+++ b/templates/Tray_Summary_Template.xlsx
@@ -1,98 +1,92 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FAswing\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CBE6F6-1DEA-483C-AEAD-1947C66DD05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
-  <si>
-    <t>BP</t>
-  </si>
-  <si>
-    <t>FRESH</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
-    <fill>
-      <patternFill patternType="none"/>
+  <fills count="9">
+    <fill>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0090EE90"/>
+        <bgColor rgb="0090EE90"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ADD8E6"/>
+        <bgColor rgb="00ADD8E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFCC"/>
+        <bgColor rgb="00FFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -115,38 +109,152 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -412,72 +520,138 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="20.77734375" customWidth="1" style="5" min="9" max="9"/>
+    <col width="18.33203125" customWidth="1" style="5" min="10" max="10"/>
+    <col width="16.6640625" customWidth="1" style="5" min="11" max="11"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+    <row r="1">
+      <c r="A1" s="4" t="n"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
+    <row r="2">
+      <c r="A2" s="16" t="n"/>
+      <c r="B2" s="17" t="inlineStr">
+        <is>
+          <t>BP</t>
+        </is>
+      </c>
+      <c r="C2" s="17" t="inlineStr">
+        <is>
+          <t>FRESH</t>
+        </is>
+      </c>
+      <c r="D2" s="17" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="F2" s="18" t="inlineStr">
+        <is>
+          <t>SN</t>
+        </is>
+      </c>
+      <c r="G2" s="18" t="inlineStr">
+        <is>
+          <t>BP</t>
+        </is>
+      </c>
+      <c r="H2" s="18" t="inlineStr">
+        <is>
+          <t>RESULT</t>
+        </is>
+      </c>
+      <c r="I2" s="18" t="inlineStr">
+        <is>
+          <t>PART_NUMBER</t>
+        </is>
+      </c>
+      <c r="J2" s="18" t="inlineStr">
+        <is>
+          <t>LAST_STATION</t>
+        </is>
+      </c>
+      <c r="K2" s="18" t="inlineStr">
+        <is>
+          <t>LAST_TEST_TIME</t>
+        </is>
+      </c>
+      <c r="L2" s="18" t="inlineStr">
+        <is>
+          <t>ERROR_CODE</t>
+        </is>
+      </c>
+      <c r="M2" s="18" t="inlineStr">
+        <is>
+          <t>FAILURE_MSG</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
+    <row r="3">
+      <c r="A3" s="17" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B3" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="16" t="n"/>
+      <c r="G3" s="16" t="n"/>
+      <c r="H3" s="16" t="n"/>
+      <c r="I3" s="16" t="n"/>
+      <c r="J3" s="16" t="n"/>
+      <c r="K3" s="16" t="n"/>
+      <c r="L3" s="16" t="n"/>
+      <c r="M3" s="16" t="n"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
+    <row r="4">
+      <c r="A4" s="17" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="B4" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="19" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
+    <row r="5">
+      <c r="A5" s="17" t="inlineStr">
+        <is>
+          <t>FAIL</t>
+        </is>
+      </c>
+      <c r="B5" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -486,5 +660,6 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>